<commit_message>
空き待ちリスト、トラブル一覧 Signed-off-by: LiuYiYang <lyy@shequchina.cn>
</commit_message>
<xml_diff>
--- a/test_物件管理/test_契約管理_随時対応（保管場、値上げ）.xlsx
+++ b/test_物件管理/test_契約管理_随時対応（保管場、値上げ）.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4506"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="165" windowWidth="14805" windowHeight="7950" tabRatio="758" firstSheet="11" activeTab="13"/>
+    <workbookView xWindow="240" yWindow="165" windowWidth="14805" windowHeight="7950" tabRatio="758"/>
   </bookViews>
   <sheets>
     <sheet name="IN_DB_001" sheetId="7" r:id="rId1"/>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10770" uniqueCount="1077">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10769" uniqueCount="1077">
   <si>
     <t>URL:</t>
   </si>
@@ -5160,8 +5160,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:IE122"/>
   <sheetViews>
-    <sheetView topLeftCell="A19" workbookViewId="0">
-      <selection activeCell="C13" sqref="C13"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F14" sqref="F14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5"/>
@@ -5282,11 +5282,11 @@
         <v>658</v>
       </c>
     </row>
-    <row r="17" spans="1:2" s="71" customFormat="1" ht="14.25">
+    <row r="17" spans="1:6" s="71" customFormat="1" ht="14.25">
       <c r="A17" s="74"/>
       <c r="B17" s="49"/>
     </row>
-    <row r="18" spans="1:2" s="71" customFormat="1" ht="14.25">
+    <row r="18" spans="1:6" s="71" customFormat="1" ht="14.25">
       <c r="A18" s="74" t="s">
         <v>165</v>
       </c>
@@ -5294,7 +5294,7 @@
         <v>639</v>
       </c>
     </row>
-    <row r="19" spans="1:2" s="64" customFormat="1" ht="14.25">
+    <row r="19" spans="1:6" s="64" customFormat="1" ht="14.25">
       <c r="A19" s="40" t="s">
         <v>165</v>
       </c>
@@ -5302,19 +5302,20 @@
         <v>659</v>
       </c>
     </row>
-    <row r="20" spans="1:2" s="50" customFormat="1">
+    <row r="20" spans="1:6" s="50" customFormat="1">
       <c r="A20" s="32"/>
       <c r="B20" s="49"/>
     </row>
-    <row r="21" spans="1:2" s="32" customFormat="1" ht="14.25">
+    <row r="21" spans="1:6" s="32" customFormat="1" ht="14.25">
       <c r="A21" s="17" t="s">
         <v>165</v>
       </c>
       <c r="B21" s="49" t="s">
         <v>661</v>
       </c>
-    </row>
-    <row r="22" spans="1:2" s="32" customFormat="1" ht="14.25">
+      <c r="F21" s="185"/>
+    </row>
+    <row r="22" spans="1:6" s="32" customFormat="1" ht="14.25">
       <c r="A22" s="17" t="s">
         <v>165</v>
       </c>
@@ -5322,10 +5323,10 @@
         <v>662</v>
       </c>
     </row>
-    <row r="23" spans="1:2" s="32" customFormat="1">
+    <row r="23" spans="1:6" s="32" customFormat="1">
       <c r="B23" s="49"/>
     </row>
-    <row r="24" spans="1:2" s="32" customFormat="1" ht="14.25">
+    <row r="24" spans="1:6" s="32" customFormat="1" ht="14.25">
       <c r="A24" s="74" t="s">
         <v>165</v>
       </c>
@@ -5333,7 +5334,7 @@
         <v>643</v>
       </c>
     </row>
-    <row r="25" spans="1:2" s="71" customFormat="1" ht="14.25">
+    <row r="25" spans="1:6" s="71" customFormat="1" ht="14.25">
       <c r="A25" s="74" t="s">
         <v>165</v>
       </c>
@@ -5341,7 +5342,7 @@
         <v>644</v>
       </c>
     </row>
-    <row r="26" spans="1:2" s="32" customFormat="1" ht="14.25">
+    <row r="26" spans="1:6" s="32" customFormat="1" ht="14.25">
       <c r="A26" s="17" t="s">
         <v>165</v>
       </c>
@@ -5349,11 +5350,11 @@
         <v>640</v>
       </c>
     </row>
-    <row r="27" spans="1:2" s="71" customFormat="1" ht="14.25">
+    <row r="27" spans="1:6" s="71" customFormat="1" ht="14.25">
       <c r="A27" s="74"/>
       <c r="B27" s="49"/>
     </row>
-    <row r="28" spans="1:2" s="71" customFormat="1" ht="14.25">
+    <row r="28" spans="1:6" s="71" customFormat="1" ht="14.25">
       <c r="A28" s="74" t="s">
         <v>165</v>
       </c>
@@ -5361,7 +5362,7 @@
         <v>648</v>
       </c>
     </row>
-    <row r="29" spans="1:2" s="71" customFormat="1" ht="14.25">
+    <row r="29" spans="1:6" s="71" customFormat="1" ht="14.25">
       <c r="A29" s="74" t="s">
         <v>165</v>
       </c>
@@ -5369,7 +5370,7 @@
         <v>645</v>
       </c>
     </row>
-    <row r="30" spans="1:2" s="71" customFormat="1" ht="14.25">
+    <row r="30" spans="1:6" s="71" customFormat="1" ht="14.25">
       <c r="A30" s="74" t="s">
         <v>165</v>
       </c>
@@ -5377,7 +5378,7 @@
         <v>647</v>
       </c>
     </row>
-    <row r="31" spans="1:2" s="71" customFormat="1" ht="14.25">
+    <row r="31" spans="1:6" s="71" customFormat="1" ht="14.25">
       <c r="A31" s="74" t="s">
         <v>165</v>
       </c>
@@ -5385,7 +5386,7 @@
         <v>646</v>
       </c>
     </row>
-    <row r="32" spans="1:2" ht="14.25">
+    <row r="32" spans="1:6" ht="14.25">
       <c r="A32" s="74" t="s">
         <v>165</v>
       </c>
@@ -25146,7 +25147,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:EL43"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="CL1" workbookViewId="0">
+    <sheetView topLeftCell="CL1" workbookViewId="0">
       <selection activeCell="CQ19" sqref="CQ19"/>
     </sheetView>
   </sheetViews>

</xml_diff>